<commit_message>
aligned times and dates
</commit_message>
<xml_diff>
--- a/Coding Journal.xlsx
+++ b/Coding Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\code-journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED06E26C-E8AD-42AF-897C-9ACA53E0B7CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F294CC11-D92B-4A25-B921-F856976AC853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0F29D09F-9D0B-41A5-94DD-0AFA6B7AA807}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="97">
   <si>
     <t>Day</t>
   </si>
@@ -251,9 +251,6 @@
     <t>Learning Command Line:
 https://www.learnenough.com/command-line-tutorial
 Backing up and wiping Rikaela’s laptop</t>
-  </si>
-  <si>
-    <t>Wiping and updating Rikaela’s laptop</t>
   </si>
   <si>
     <t>Decrypting Rikaela’s laptop
@@ -486,10 +483,6 @@
 Regular Expressions - 1 new lesson
 Ended on:
 https://www.freecodecamp.org/learn/javascript-algorithms-and-data-structures/javascript-algorithms-and-data-structures-projects/cash-register</t>
-  </si>
-  <si>
-    <t>Cash Register Project
-Claimed the JavaScript Algorithms and Data Structures Certification in 30 days - 39.5 hrs/300</t>
   </si>
   <si>
     <t>Front End Libraries Certification:
@@ -687,12 +680,28 @@
   <si>
     <t>Front End Libraries Certification:
 Quote Machine
-Added ability to tweet quote, added comments, cleaned up code, uploaded to GitHub</t>
+Downlaoded Postman to view API data, added API call to get quote and author</t>
   </si>
   <si>
     <t>Front End Libraries Certification:
 Quote Machine
-Downlaoded Postman to view API data, added API call to get quote and author</t>
+Added ability to tweet quote, added comments, cleaned up code, uploaded to GitHub
+Uploaded old projects to GitHub</t>
+  </si>
+  <si>
+    <t>8/2/2018-
+8/7/2018</t>
+  </si>
+  <si>
+    <t>8/9/2018-
+2/25/2020</t>
+  </si>
+  <si>
+    <t>Team/role changes at work</t>
+  </si>
+  <si>
+    <t>Cash Register Project
+Claimed the JavaScript Algorithms and Data Structures Certification in 40 days - 49.25 hrs/300</t>
   </si>
 </sst>
 </file>
@@ -785,7 +794,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -819,6 +828,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1136,10 +1148,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D76F79-11B2-4973-A532-DBF6DFAAF042}">
-  <dimension ref="A1:D123"/>
+  <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="D123" sqref="D123"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="H91" sqref="H91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1697,26 +1709,26 @@
         <v>36</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
       <c r="B40" s="2">
-        <v>43274</v>
+        <v>43275</v>
       </c>
       <c r="C40" s="1">
         <v>1</v>
       </c>
-      <c r="D40" s="3" t="s">
+      <c r="D40" s="9" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>40</v>
       </c>
       <c r="B41" s="2">
-        <v>43275</v>
+        <v>43276</v>
       </c>
       <c r="C41" s="1">
         <v>1</v>
@@ -1730,13 +1742,13 @@
         <v>41</v>
       </c>
       <c r="B42" s="2">
-        <v>43276</v>
+        <v>43277</v>
       </c>
       <c r="C42" s="1">
         <v>1</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1744,40 +1756,40 @@
         <v>42</v>
       </c>
       <c r="B43" s="2">
-        <v>43277</v>
+        <v>43278</v>
       </c>
       <c r="C43" s="1">
         <v>1</v>
       </c>
-      <c r="D43" s="9" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="D43" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43</v>
       </c>
       <c r="B44" s="2">
-        <v>43278</v>
+        <v>43279</v>
       </c>
       <c r="C44" s="1">
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>44</v>
       </c>
       <c r="B45" s="2">
-        <v>43279</v>
+        <v>43280</v>
       </c>
       <c r="C45" s="1">
         <v>1</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="9" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1786,13 +1798,13 @@
         <v>45</v>
       </c>
       <c r="B46" s="2">
-        <v>43280</v>
+        <v>43281</v>
       </c>
       <c r="C46" s="1">
         <v>1</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1800,13 +1812,13 @@
         <v>46</v>
       </c>
       <c r="B47" s="2">
-        <v>43281</v>
+        <v>43282</v>
       </c>
       <c r="C47" s="1">
         <v>1</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1814,7 +1826,7 @@
         <v>47</v>
       </c>
       <c r="B48" s="2">
-        <v>43282</v>
+        <v>43283</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
@@ -1828,13 +1840,13 @@
         <v>48</v>
       </c>
       <c r="B49" s="2">
-        <v>43283</v>
+        <v>43284</v>
       </c>
       <c r="C49" s="1">
         <v>1</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1842,13 +1854,13 @@
         <v>49</v>
       </c>
       <c r="B50" s="2">
-        <v>43284</v>
+        <v>43285</v>
       </c>
       <c r="C50" s="1">
         <v>1</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1856,80 +1868,80 @@
         <v>50</v>
       </c>
       <c r="B51" s="2">
-        <v>43285</v>
+        <v>43286</v>
       </c>
       <c r="C51" s="1">
         <v>1</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>51</v>
       </c>
       <c r="B52" s="2">
-        <v>43286</v>
+        <v>43287</v>
       </c>
       <c r="C52" s="1">
-        <v>1</v>
-      </c>
-      <c r="D52" s="9" t="s">
+        <v>1.75</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>52</v>
       </c>
       <c r="B53" s="2">
-        <v>43287</v>
+        <v>43288</v>
       </c>
       <c r="C53" s="1">
-        <v>1.75</v>
+        <v>1</v>
       </c>
       <c r="D53" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>53</v>
       </c>
       <c r="B54" s="2">
-        <v>43288</v>
+        <v>43289</v>
       </c>
       <c r="C54" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D54" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
       <c r="B55" s="2">
-        <v>43289</v>
+        <v>43290</v>
       </c>
       <c r="C55" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>55</v>
       </c>
       <c r="B56" s="2">
-        <v>43290</v>
+        <v>43291</v>
       </c>
       <c r="C56" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>46</v>
@@ -1940,10 +1952,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="2">
-        <v>43291</v>
+        <v>43292</v>
       </c>
       <c r="C57" s="1">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>47</v>
@@ -1954,13 +1966,13 @@
         <v>57</v>
       </c>
       <c r="B58" s="2">
-        <v>43292</v>
+        <v>43293</v>
       </c>
       <c r="C58" s="1">
         <v>1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1968,7 +1980,7 @@
         <v>58</v>
       </c>
       <c r="B59" s="2">
-        <v>43293</v>
+        <v>43294</v>
       </c>
       <c r="C59" s="1">
         <v>1</v>
@@ -1982,13 +1994,13 @@
         <v>59</v>
       </c>
       <c r="B60" s="2">
-        <v>43294</v>
+        <v>43295</v>
       </c>
       <c r="C60" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1996,13 +2008,13 @@
         <v>60</v>
       </c>
       <c r="B61" s="2">
-        <v>43295</v>
+        <v>43296</v>
       </c>
       <c r="C61" s="1">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2010,7 +2022,7 @@
         <v>61</v>
       </c>
       <c r="B62" s="2">
-        <v>43296</v>
+        <v>43297</v>
       </c>
       <c r="C62" s="1">
         <v>1</v>
@@ -2024,13 +2036,13 @@
         <v>62</v>
       </c>
       <c r="B63" s="2">
-        <v>43297</v>
+        <v>43298</v>
       </c>
       <c r="C63" s="1">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2038,13 +2050,13 @@
         <v>63</v>
       </c>
       <c r="B64" s="2">
-        <v>43298</v>
+        <v>43299</v>
       </c>
       <c r="C64" s="1">
-        <v>2.5</v>
+        <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2052,13 +2064,13 @@
         <v>64</v>
       </c>
       <c r="B65" s="2">
-        <v>43299</v>
+        <v>43300</v>
       </c>
       <c r="C65" s="1">
         <v>1</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2066,13 +2078,13 @@
         <v>65</v>
       </c>
       <c r="B66" s="2">
-        <v>43300</v>
+        <v>43301</v>
       </c>
       <c r="C66" s="1">
         <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2080,13 +2092,13 @@
         <v>66</v>
       </c>
       <c r="B67" s="2">
-        <v>43301</v>
+        <v>43302</v>
       </c>
       <c r="C67" s="1">
-        <v>1</v>
+        <v>1.5</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2094,13 +2106,13 @@
         <v>67</v>
       </c>
       <c r="B68" s="2">
-        <v>43302</v>
+        <v>43303</v>
       </c>
       <c r="C68" s="1">
-        <v>1.5</v>
+        <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2108,13 +2120,13 @@
         <v>68</v>
       </c>
       <c r="B69" s="2">
-        <v>43303</v>
+        <v>43304</v>
       </c>
       <c r="C69" s="1">
         <v>1</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2122,13 +2134,13 @@
         <v>69</v>
       </c>
       <c r="B70" s="2">
-        <v>43304</v>
+        <v>43305</v>
       </c>
       <c r="C70" s="1">
-        <v>1</v>
+        <v>1.25</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2136,10 +2148,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="2">
-        <v>43305</v>
+        <v>43306</v>
       </c>
       <c r="C71" s="1">
-        <v>1.25</v>
+        <v>1</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>50</v>
@@ -2150,13 +2162,13 @@
         <v>71</v>
       </c>
       <c r="B72" s="2">
-        <v>43306</v>
+        <v>43307</v>
       </c>
       <c r="C72" s="1">
         <v>1</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2164,13 +2176,13 @@
         <v>72</v>
       </c>
       <c r="B73" s="2">
-        <v>43307</v>
+        <v>43311</v>
       </c>
       <c r="C73" s="1">
         <v>1</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2178,13 +2190,13 @@
         <v>73</v>
       </c>
       <c r="B74" s="2">
-        <v>43311</v>
+        <v>43312</v>
       </c>
       <c r="C74" s="1">
         <v>1</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2192,7 +2204,7 @@
         <v>74</v>
       </c>
       <c r="B75" s="2">
-        <v>43312</v>
+        <v>43313</v>
       </c>
       <c r="C75" s="1">
         <v>1</v>
@@ -2202,25 +2214,21 @@
       </c>
     </row>
     <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="1">
-        <v>75</v>
-      </c>
-      <c r="B76" s="2">
-        <v>43313</v>
-      </c>
-      <c r="C76" s="1">
-        <v>1</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="C76" s="1"/>
       <c r="D76" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" s="2">
-        <v>43314</v>
+        <v>43320</v>
       </c>
       <c r="C77" s="1">
         <v>1</v>
@@ -2229,648 +2237,574 @@
         <v>53</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="1">
+    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="C78" s="1"/>
+      <c r="D78" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A79" s="1">
+        <v>76</v>
+      </c>
+      <c r="B79" s="2">
+        <v>43886</v>
+      </c>
+      <c r="C79" s="1">
+        <v>1</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A80" s="1">
         <v>77</v>
       </c>
-      <c r="B78" s="2">
-        <v>43315</v>
-      </c>
-      <c r="C78" s="1">
-        <v>1</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="1">
+      <c r="B80" s="2">
+        <v>43887</v>
+      </c>
+      <c r="C80" s="1">
+        <v>1</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A81" s="1">
         <v>78</v>
       </c>
-      <c r="B79" s="2">
-        <v>43316</v>
-      </c>
-      <c r="C79" s="1">
-        <v>1</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="1">
+      <c r="B81" s="2">
+        <v>43888</v>
+      </c>
+      <c r="C81" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A82" s="1">
         <v>79</v>
       </c>
-      <c r="B80" s="2">
-        <v>43317</v>
-      </c>
-      <c r="C80" s="1">
-        <v>1</v>
-      </c>
-      <c r="D80" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" s="1">
+      <c r="B82" s="2">
+        <v>43889</v>
+      </c>
+      <c r="C82" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="D82" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A83" s="1">
         <v>80</v>
       </c>
-      <c r="B81" s="2">
-        <v>43318</v>
-      </c>
-      <c r="C81" s="1">
-        <v>1</v>
-      </c>
-      <c r="D81" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="1">
+      <c r="B83" s="2">
+        <v>43890</v>
+      </c>
+      <c r="C83" s="1">
+        <v>2</v>
+      </c>
+      <c r="D83" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" ht="165" x14ac:dyDescent="0.25">
+      <c r="A84" s="1">
         <v>81</v>
       </c>
-      <c r="B82" s="2">
-        <v>43319</v>
-      </c>
-      <c r="C82" s="1">
-        <v>1</v>
-      </c>
-      <c r="D82" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A83" s="1">
-        <v>82</v>
-      </c>
-      <c r="B83" s="2">
-        <v>43320</v>
-      </c>
-      <c r="C83" s="1">
-        <v>1</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A84" s="1">
-        <v>83</v>
-      </c>
       <c r="B84" s="2">
-        <v>43886</v>
+        <v>43891</v>
       </c>
       <c r="C84" s="1">
-        <v>1</v>
+        <v>1.75</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B85" s="2">
-        <v>43887</v>
+        <v>43892</v>
       </c>
       <c r="C85" s="1">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B86" s="2">
-        <v>43888</v>
+        <v>43893</v>
       </c>
       <c r="C86" s="1">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
+        <v>84</v>
+      </c>
+      <c r="B87" s="5">
+        <v>43894</v>
+      </c>
+      <c r="C87" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D87" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A88" s="1">
+        <v>85</v>
+      </c>
+      <c r="B88" s="5">
+        <v>43895</v>
+      </c>
+      <c r="C88" s="4">
+        <v>1</v>
+      </c>
+      <c r="D88" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A89" s="1">
         <v>86</v>
       </c>
-      <c r="B87" s="2">
-        <v>43889</v>
-      </c>
-      <c r="C87" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="D87" s="3" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="88" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A88" s="1">
-        <v>87</v>
-      </c>
-      <c r="B88" s="2">
-        <v>43890</v>
-      </c>
-      <c r="C88" s="1">
-        <v>2</v>
-      </c>
-      <c r="D88" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="89" spans="1:4" ht="165" x14ac:dyDescent="0.25">
-      <c r="A89" s="1">
-        <v>88</v>
-      </c>
-      <c r="B89" s="2">
-        <v>43891</v>
-      </c>
-      <c r="C89" s="1">
-        <v>1.75</v>
-      </c>
-      <c r="D89" s="3" t="s">
-        <v>60</v>
+      <c r="B89" s="5">
+        <v>43896</v>
+      </c>
+      <c r="C89" s="4">
+        <v>1</v>
+      </c>
+      <c r="D89" s="6" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
-        <v>89</v>
-      </c>
-      <c r="B90" s="2">
-        <v>43892</v>
-      </c>
-      <c r="C90" s="1">
-        <v>0.75</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>61</v>
+        <v>87</v>
+      </c>
+      <c r="B90" s="5">
+        <v>43897</v>
+      </c>
+      <c r="C90" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D90" s="6" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="150" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
+        <v>88</v>
+      </c>
+      <c r="B91" s="5">
+        <v>43898</v>
+      </c>
+      <c r="C91" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A92" s="1">
+        <v>89</v>
+      </c>
+      <c r="B92" s="5">
+        <v>43899</v>
+      </c>
+      <c r="C92" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A93" s="1">
         <v>90</v>
       </c>
-      <c r="B91" s="2">
-        <v>43893</v>
-      </c>
-      <c r="C91" s="1">
-        <v>1</v>
-      </c>
-      <c r="D91" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A92" s="4">
+      <c r="B93" s="5">
+        <v>43900</v>
+      </c>
+      <c r="C93" s="4">
+        <v>2.75</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A94" s="1">
         <v>91</v>
       </c>
-      <c r="B92" s="5">
-        <v>43894</v>
-      </c>
-      <c r="C92" s="4">
+      <c r="B94" s="11">
+        <v>43901</v>
+      </c>
+      <c r="C94" s="10">
+        <v>3</v>
+      </c>
+      <c r="D94" s="12" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A95" s="1">
+        <v>92</v>
+      </c>
+      <c r="B95" s="5">
+        <v>43902</v>
+      </c>
+      <c r="C95" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A96" s="1">
+        <v>93</v>
+      </c>
+      <c r="B96" s="5">
+        <v>43903</v>
+      </c>
+      <c r="C96" s="4">
         <v>0.5</v>
       </c>
-      <c r="D92" s="6" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A93" s="4">
-        <v>92</v>
-      </c>
-      <c r="B93" s="5">
-        <v>43895</v>
-      </c>
-      <c r="C93" s="4">
-        <v>1</v>
-      </c>
-      <c r="D93" s="6" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A94" s="4">
-        <v>93</v>
-      </c>
-      <c r="B94" s="5">
-        <v>43896</v>
-      </c>
-      <c r="C94" s="4">
-        <v>1</v>
-      </c>
-      <c r="D94" s="6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="95" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A95" s="4">
+      <c r="D96" s="6" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A97" s="1">
         <v>94</v>
       </c>
-      <c r="B95" s="5">
-        <v>43897</v>
-      </c>
-      <c r="C95" s="4">
+      <c r="B97" s="5">
+        <v>43904</v>
+      </c>
+      <c r="C97" s="4">
+        <v>1</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A98" s="1">
+        <v>95</v>
+      </c>
+      <c r="B98" s="5">
+        <v>43905</v>
+      </c>
+      <c r="C98" s="4">
+        <v>1</v>
+      </c>
+      <c r="D98" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A99" s="1">
+        <v>96</v>
+      </c>
+      <c r="B99" s="5">
+        <v>43906</v>
+      </c>
+      <c r="C99" s="4">
+        <v>1</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100" s="1">
+        <v>97</v>
+      </c>
+      <c r="B100" s="5">
+        <v>43907</v>
+      </c>
+      <c r="C100" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A101" s="1">
+        <v>98</v>
+      </c>
+      <c r="B101" s="5">
+        <v>43908</v>
+      </c>
+      <c r="C101" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A102" s="1">
+        <v>99</v>
+      </c>
+      <c r="B102" s="5">
+        <v>43909</v>
+      </c>
+      <c r="C102" s="4">
         <v>0.5</v>
       </c>
-      <c r="D95" s="6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A96" s="4">
-        <v>95</v>
-      </c>
-      <c r="B96" s="5">
-        <v>43898</v>
-      </c>
-      <c r="C96" s="4">
-        <v>2.5</v>
-      </c>
-      <c r="D96" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="97" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A97" s="4">
-        <v>96</v>
-      </c>
-      <c r="B97" s="5">
-        <v>43899</v>
-      </c>
-      <c r="C97" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D97" s="6" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="98" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A98" s="4">
-        <v>97</v>
-      </c>
-      <c r="B98" s="5">
-        <v>43900</v>
-      </c>
-      <c r="C98" s="4">
-        <v>2.75</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="99" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A99" s="10">
-        <v>98</v>
-      </c>
-      <c r="B99" s="11">
-        <v>43901</v>
-      </c>
-      <c r="C99" s="10">
-        <v>3</v>
-      </c>
-      <c r="D99" s="12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A100" s="4">
-        <v>99</v>
-      </c>
-      <c r="B100" s="5">
-        <v>43902</v>
-      </c>
-      <c r="C100" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D100" s="6" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="101" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A101" s="4">
+      <c r="D102" s="6" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A103" s="1">
         <v>100</v>
       </c>
-      <c r="B101" s="5">
-        <v>43903</v>
-      </c>
-      <c r="C101" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D101" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="102" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A102" s="4">
+      <c r="B103" s="5">
+        <v>43911</v>
+      </c>
+      <c r="C103" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" ht="150" x14ac:dyDescent="0.25">
+      <c r="A104" s="1">
         <v>101</v>
       </c>
-      <c r="B102" s="5">
-        <v>43904</v>
-      </c>
-      <c r="C102" s="4">
-        <v>1</v>
-      </c>
-      <c r="D102" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="103" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A103" s="4">
+      <c r="B104" s="5">
+        <v>43912</v>
+      </c>
+      <c r="C104" s="4">
+        <v>1</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="105" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A105" s="1">
         <v>102</v>
       </c>
-      <c r="B103" s="5">
-        <v>43905</v>
-      </c>
-      <c r="C103" s="4">
-        <v>1</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="104" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A104" s="4">
+      <c r="B105" s="5">
+        <v>43913</v>
+      </c>
+      <c r="C105" s="4">
+        <v>1</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A106" s="1">
         <v>103</v>
       </c>
-      <c r="B104" s="5">
-        <v>43906</v>
-      </c>
-      <c r="C104" s="4">
-        <v>1</v>
-      </c>
-      <c r="D104" s="6" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="105" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A105" s="4">
+      <c r="B106" s="5">
+        <v>43914</v>
+      </c>
+      <c r="C106" s="4">
+        <v>1</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A107" s="1">
         <v>104</v>
       </c>
-      <c r="B105" s="5">
-        <v>43907</v>
-      </c>
-      <c r="C105" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D105" s="6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="106" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A106" s="4">
-        <v>105</v>
-      </c>
-      <c r="B106" s="5">
-        <v>43908</v>
-      </c>
-      <c r="C106" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D106" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="107" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A107" s="4">
-        <v>106</v>
-      </c>
       <c r="B107" s="5">
-        <v>43909</v>
+        <v>43915</v>
       </c>
       <c r="C107" s="4">
         <v>0.5</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="108" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A108" s="4">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A108" s="1">
+        <v>105</v>
+      </c>
+      <c r="B108" s="5">
+        <v>43917</v>
+      </c>
+      <c r="C108" s="4">
+        <v>1</v>
+      </c>
+      <c r="D108" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A109" s="1">
+        <v>106</v>
+      </c>
+      <c r="B109" s="5">
+        <v>43918</v>
+      </c>
+      <c r="C109" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="D109" s="6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A110" s="1">
         <v>107</v>
       </c>
-      <c r="B108" s="5">
-        <v>43911</v>
-      </c>
-      <c r="C108" s="4">
+      <c r="B110" s="5">
+        <v>43920</v>
+      </c>
+      <c r="C110" s="4">
         <v>1.5</v>
       </c>
-      <c r="D108" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="109" spans="1:4" ht="150" x14ac:dyDescent="0.25">
-      <c r="A109" s="4">
+      <c r="D110" s="6" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A111" s="1">
         <v>108</v>
       </c>
-      <c r="B109" s="5">
-        <v>43912</v>
-      </c>
-      <c r="C109" s="4">
-        <v>1</v>
-      </c>
-      <c r="D109" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="110" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A110" s="4">
+      <c r="B111" s="5">
+        <v>43921</v>
+      </c>
+      <c r="C111" s="4">
+        <v>1</v>
+      </c>
+      <c r="D111" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A112" s="1">
         <v>109</v>
       </c>
-      <c r="B110" s="5">
-        <v>43913</v>
-      </c>
-      <c r="C110" s="4">
-        <v>1</v>
-      </c>
-      <c r="D110" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="111" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A111" s="4">
+      <c r="B112" s="5">
+        <v>43922</v>
+      </c>
+      <c r="C112" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D112" s="6" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A113" s="1">
         <v>110</v>
       </c>
-      <c r="B111" s="5">
-        <v>43914</v>
-      </c>
-      <c r="C111" s="4">
-        <v>1</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="112" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A112" s="4">
+      <c r="B113" s="5">
+        <v>43923</v>
+      </c>
+      <c r="C113" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D113" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A114" s="1">
         <v>111</v>
       </c>
-      <c r="B112" s="5">
-        <v>43915</v>
-      </c>
-      <c r="C112" s="4">
-        <v>0.5</v>
-      </c>
-      <c r="D112" s="6" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A113" s="4">
-        <v>112</v>
-      </c>
-      <c r="B113" s="5">
-        <v>43917</v>
-      </c>
-      <c r="C113" s="4">
-        <v>1</v>
-      </c>
-      <c r="D113" s="6" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A114" s="4">
-        <v>113</v>
-      </c>
       <c r="B114" s="5">
-        <v>43918</v>
+        <v>43926</v>
       </c>
       <c r="C114" s="4">
         <v>1.5</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A115" s="4">
+      <c r="A115" s="1">
+        <v>112</v>
+      </c>
+      <c r="B115" s="5">
+        <v>43927</v>
+      </c>
+      <c r="C115" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="D115" s="6" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A116" s="1">
+        <v>113</v>
+      </c>
+      <c r="B116" s="5">
+        <v>43928</v>
+      </c>
+      <c r="C116" s="4">
+        <v>1</v>
+      </c>
+      <c r="D116" s="6" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A117" s="1">
         <v>114</v>
       </c>
-      <c r="B115" s="5">
-        <v>43920</v>
-      </c>
-      <c r="C115" s="4">
+      <c r="B117" s="5">
+        <v>43929</v>
+      </c>
+      <c r="C117" s="4">
+        <v>1</v>
+      </c>
+      <c r="D117" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A118" s="1">
+        <v>115</v>
+      </c>
+      <c r="B118" s="5">
+        <v>43930</v>
+      </c>
+      <c r="C118" s="4">
         <v>1.5</v>
       </c>
-      <c r="D115" s="6" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="116" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A116" s="4">
-        <v>115</v>
-      </c>
-      <c r="B116" s="5">
-        <v>43921</v>
-      </c>
-      <c r="C116" s="4">
-        <v>1</v>
-      </c>
-      <c r="D116" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="117" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A117" s="4">
-        <v>116</v>
-      </c>
-      <c r="B117" s="5">
-        <v>43922</v>
-      </c>
-      <c r="C117" s="4">
-        <v>0.75</v>
-      </c>
-      <c r="D117" s="6" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="118" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A118" s="4">
-        <v>117</v>
-      </c>
-      <c r="B118" s="5">
-        <v>43923</v>
-      </c>
-      <c r="C118" s="4">
-        <v>0.75</v>
-      </c>
       <c r="D118" s="6" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="119" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A119" s="4">
-        <v>118</v>
-      </c>
-      <c r="B119" s="5">
-        <v>43926</v>
-      </c>
-      <c r="C119" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D119" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A120" s="4">
-        <v>119</v>
-      </c>
-      <c r="B120" s="5">
-        <v>43927</v>
-      </c>
-      <c r="C120" s="4">
-        <v>1.25</v>
-      </c>
-      <c r="D120" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="121" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A121" s="4">
-        <v>120</v>
-      </c>
-      <c r="B121" s="5">
-        <v>43928</v>
-      </c>
-      <c r="C121" s="4">
-        <v>1</v>
-      </c>
-      <c r="D121" s="6" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="122" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A122" s="4">
-        <v>121</v>
-      </c>
-      <c r="B122" s="5">
-        <v>43929</v>
-      </c>
-      <c r="C122" s="4">
-        <v>1</v>
-      </c>
-      <c r="D122" s="6" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="123" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A123" s="4">
-        <v>122</v>
-      </c>
-      <c r="B123" s="5">
-        <v>43930</v>
-      </c>
-      <c r="C123" s="4">
-        <v>1.5</v>
-      </c>
-      <c r="D123" s="6" t="s">
-        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -2893,17 +2827,17 @@
     <hyperlink ref="D30" r:id="rId16" display="https://www.freecodecamp.org/certification/fcc7c519116-363d-4e4c-8a88-dbce18860629/responsive-web-design" xr:uid="{95DCB9D4-7D4C-4555-8FEE-43E673A8B69B}"/>
     <hyperlink ref="D37" r:id="rId17" display="https://www.theodinproject.com/courses/web-development-101/lessons/git-basics" xr:uid="{3BB6BA5B-4695-4E3A-A6B3-CC0DE9682158}"/>
     <hyperlink ref="D39" r:id="rId18" display="https://www.learnenough.com/command-line-tutorial" xr:uid="{3A54F693-19E9-4E9C-AFB4-3C235AAD7A46}"/>
-    <hyperlink ref="D41" r:id="rId19" display="https://www.learnenough.com/command-line-tutorial" xr:uid="{22672B4C-2E39-4A97-B81A-0B920F185504}"/>
-    <hyperlink ref="D42" r:id="rId20" display="https://www.learnenough.com/command-line-tutorial" xr:uid="{94447611-24CA-4C6A-A33B-537C1644EF94}"/>
-    <hyperlink ref="D43" r:id="rId21" display="https://www.learnenough.com/command-line-tutorial" xr:uid="{EFF4E555-D09F-4860-B098-D7725E39F57A}"/>
-    <hyperlink ref="D46" r:id="rId22" display="https://www.learnenough.com/text-editor-tutorial" xr:uid="{663F3BAC-D290-4B4B-A8E2-02A82795C73F}"/>
-    <hyperlink ref="D47" r:id="rId23" display="https://www.learnenough.com/text-editor-tutorial" xr:uid="{E469824E-AC0C-4FED-8A8C-D50FCF6D8A58}"/>
-    <hyperlink ref="D48" r:id="rId24" display="https://www.learnenough.com/text-editor-tutorial" xr:uid="{F751FFA5-DD8E-4751-8B8D-8711F4ACFAD5}"/>
-    <hyperlink ref="D49" r:id="rId25" display="https://www.learnenough.com/git-tutorial" xr:uid="{3F998587-338E-4859-B0A8-00C51CF5DC50}"/>
-    <hyperlink ref="D50" r:id="rId26" display="https://www.learnenough.com/git-tutorial" xr:uid="{530C660B-C71F-480D-AE3A-19D5ED603EAB}"/>
-    <hyperlink ref="D51" r:id="rId27" display="https://www.learnenough.com/git-tutorial" xr:uid="{59D6F83D-4914-4128-A4DB-05DFBA9F2AD9}"/>
-    <hyperlink ref="D52" r:id="rId28" display="https://www.learnenough.com/git-tutorial" xr:uid="{6DA5A5AC-5FB2-4AFC-9941-C0ED506A3CE3}"/>
-    <hyperlink ref="D99" r:id="rId29" display="https://www.freecodecamp.org/certification/fcc7c519116-363d-4e4c-8a88-dbce18860629/javascript-algorithms-and-data-structures" xr:uid="{4B7124F9-D144-4ED5-81D8-10F3CB1B3084}"/>
+    <hyperlink ref="D40" r:id="rId19" display="https://www.learnenough.com/command-line-tutorial" xr:uid="{22672B4C-2E39-4A97-B81A-0B920F185504}"/>
+    <hyperlink ref="D41" r:id="rId20" display="https://www.learnenough.com/command-line-tutorial" xr:uid="{94447611-24CA-4C6A-A33B-537C1644EF94}"/>
+    <hyperlink ref="D42" r:id="rId21" display="https://www.learnenough.com/command-line-tutorial" xr:uid="{EFF4E555-D09F-4860-B098-D7725E39F57A}"/>
+    <hyperlink ref="D45" r:id="rId22" display="https://www.learnenough.com/text-editor-tutorial" xr:uid="{663F3BAC-D290-4B4B-A8E2-02A82795C73F}"/>
+    <hyperlink ref="D46" r:id="rId23" display="https://www.learnenough.com/text-editor-tutorial" xr:uid="{E469824E-AC0C-4FED-8A8C-D50FCF6D8A58}"/>
+    <hyperlink ref="D47" r:id="rId24" display="https://www.learnenough.com/text-editor-tutorial" xr:uid="{F751FFA5-DD8E-4751-8B8D-8711F4ACFAD5}"/>
+    <hyperlink ref="D48" r:id="rId25" display="https://www.learnenough.com/git-tutorial" xr:uid="{3F998587-338E-4859-B0A8-00C51CF5DC50}"/>
+    <hyperlink ref="D49" r:id="rId26" display="https://www.learnenough.com/git-tutorial" xr:uid="{530C660B-C71F-480D-AE3A-19D5ED603EAB}"/>
+    <hyperlink ref="D50" r:id="rId27" display="https://www.learnenough.com/git-tutorial" xr:uid="{59D6F83D-4914-4128-A4DB-05DFBA9F2AD9}"/>
+    <hyperlink ref="D51" r:id="rId28" display="https://www.learnenough.com/git-tutorial" xr:uid="{6DA5A5AC-5FB2-4AFC-9941-C0ED506A3CE3}"/>
+    <hyperlink ref="D94" r:id="rId29" display="https://www.freecodecamp.org/certification/fcc7c519116-363d-4e4c-8a88-dbce18860629/javascript-algorithms-and-data-structures" xr:uid="{4B7124F9-D144-4ED5-81D8-10F3CB1B3084}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId30"/>

</xml_diff>

<commit_message>
fixing a few things
</commit_message>
<xml_diff>
--- a/Coding Journal.xlsx
+++ b/Coding Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\code-journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F294CC11-D92B-4A25-B921-F856976AC853}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEC72FE9-0AB0-4B67-B084-34B5CA337F95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0F29D09F-9D0B-41A5-94DD-0AFA6B7AA807}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="94">
   <si>
     <t>Day</t>
   </si>
@@ -98,11 +98,6 @@
   <si>
     <t>Legacy Front-End Certification:
 Basic Algorithms</t>
-  </si>
-  <si>
-    <t>Legacy Front-End Certification:
-Basic Algorithms
-Completed “Chunky Monkey” &amp; “Slasher Flick” in one try, no testing</t>
   </si>
   <si>
     <t>FreeCodeCamp curriculum re-write! Going back and finishing new challenges introduced in old lessons.
@@ -249,17 +244,6 @@
   </si>
   <si>
     <t>Learning Command Line:
-https://www.learnenough.com/command-line-tutorial
-Backing up and wiping Rikaela’s laptop</t>
-  </si>
-  <si>
-    <t>Decrypting Rikaela’s laptop
-Installing iTerm2, Atom, and git
-Learning Command Line:
-https://www.learnenough.com/command-line-tutorial</t>
-  </si>
-  <si>
-    <t>Learning Command Line:
 https://www.learnenough.com/command-line-tutorial</t>
   </si>
   <si>
@@ -287,11 +271,6 @@
   <si>
     <t>JavaScript Algorithms and Data Structures Certification:
 Basic Data Structures</t>
-  </si>
-  <si>
-    <t>JavaScript Algorithms and Data Structures Certification:
-Basic Data Structures
-Re-seated Rikaela’s RAM</t>
   </si>
   <si>
     <t>JavaScript Algorithms and Data Structures Certification:
@@ -702,6 +681,11 @@
   <si>
     <t>Cash Register Project
 Claimed the JavaScript Algorithms and Data Structures Certification in 40 days - 49.25 hrs/300</t>
+  </si>
+  <si>
+    <t>Installing iTerm2, Atom, and git
+Learning Command Line:
+https://www.learnenough.com/command-line-tutorial</t>
   </si>
 </sst>
 </file>
@@ -1150,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D76F79-11B2-4973-A532-DBF6DFAAF042}">
   <dimension ref="A1:D118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H91" sqref="H91"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1359,7 +1343,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1370,7 +1354,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1384,7 +1368,7 @@
         <v>1</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1398,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1412,7 +1396,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1426,7 +1410,7 @@
         <v>1</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -1440,7 +1424,7 @@
         <v>2.5</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1454,7 +1438,7 @@
         <v>1.5</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -1468,7 +1452,7 @@
         <v>1</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -1482,7 +1466,7 @@
         <v>1</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1496,7 +1480,7 @@
         <v>1.5</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -1510,7 +1494,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="120" x14ac:dyDescent="0.25">
@@ -1524,7 +1508,7 @@
         <v>1.25</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1538,7 +1522,7 @@
         <v>1</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="120" x14ac:dyDescent="0.25">
@@ -1552,7 +1536,7 @@
         <v>1.25</v>
       </c>
       <c r="D28" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -1566,7 +1550,7 @@
         <v>1.5</v>
       </c>
       <c r="D29" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -1580,7 +1564,7 @@
         <v>1</v>
       </c>
       <c r="D30" s="12" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -1594,7 +1578,7 @@
         <v>1.75</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1608,7 +1592,7 @@
         <v>1.25</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1622,7 +1606,7 @@
         <v>1.25</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1636,7 +1620,7 @@
         <v>1</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="135" x14ac:dyDescent="0.25">
@@ -1650,7 +1634,7 @@
         <v>1.25</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1664,7 +1648,7 @@
         <v>1</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1678,7 +1662,7 @@
         <v>1</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1692,10 +1676,10 @@
         <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -1706,10 +1690,10 @@
         <v>1</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -1720,7 +1704,7 @@
         <v>1</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>37</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1734,7 +1718,7 @@
         <v>1</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1748,7 +1732,7 @@
         <v>1</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1762,7 +1746,7 @@
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1776,7 +1760,7 @@
         <v>1</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1790,7 +1774,7 @@
         <v>1</v>
       </c>
       <c r="D45" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1804,7 +1788,7 @@
         <v>1</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1818,7 +1802,7 @@
         <v>1</v>
       </c>
       <c r="D47" s="9" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1832,7 +1816,7 @@
         <v>1</v>
       </c>
       <c r="D48" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1846,7 +1830,7 @@
         <v>1</v>
       </c>
       <c r="D49" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1860,7 +1844,7 @@
         <v>1</v>
       </c>
       <c r="D50" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1874,7 +1858,7 @@
         <v>1</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -1888,7 +1872,7 @@
         <v>1.75</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -1902,7 +1886,7 @@
         <v>1</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1916,10 +1900,10 @@
         <v>0.75</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -1930,7 +1914,7 @@
         <v>1</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1944,7 +1928,7 @@
         <v>1.25</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1958,7 +1942,7 @@
         <v>1</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1972,7 +1956,7 @@
         <v>1</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1986,7 +1970,7 @@
         <v>1</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2000,7 +1984,7 @@
         <v>1.25</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2014,7 +1998,7 @@
         <v>1</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2028,7 +2012,7 @@
         <v>1</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2042,7 +2026,7 @@
         <v>2.5</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2056,7 +2040,7 @@
         <v>1</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2070,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2084,7 +2068,7 @@
         <v>1</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2098,7 +2082,7 @@
         <v>1.5</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2112,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2126,7 +2110,7 @@
         <v>1</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2140,7 +2124,7 @@
         <v>1.25</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2154,7 +2138,7 @@
         <v>1</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2168,7 +2152,7 @@
         <v>1</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2182,7 +2166,7 @@
         <v>1</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2196,7 +2180,7 @@
         <v>1</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2210,17 +2194,17 @@
         <v>1</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A76" s="1"/>
       <c r="B76" s="13" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2234,17 +2218,17 @@
         <v>1</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="1"/>
       <c r="B78" s="13" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="135" x14ac:dyDescent="0.25">
@@ -2258,7 +2242,7 @@
         <v>1</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2272,7 +2256,7 @@
         <v>1</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2286,7 +2270,7 @@
         <v>0.75</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2300,7 +2284,7 @@
         <v>0.75</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -2314,7 +2298,7 @@
         <v>2</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="165" x14ac:dyDescent="0.25">
@@ -2328,7 +2312,7 @@
         <v>1.75</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2342,7 +2326,7 @@
         <v>0.75</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2356,7 +2340,7 @@
         <v>1</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2370,7 +2354,7 @@
         <v>0.5</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2384,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2398,7 +2382,7 @@
         <v>1</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2412,7 +2396,7 @@
         <v>0.5</v>
       </c>
       <c r="D90" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2426,7 +2410,7 @@
         <v>2.5</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2440,7 +2424,7 @@
         <v>0.75</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -2454,7 +2438,7 @@
         <v>2.75</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -2468,7 +2452,7 @@
         <v>3</v>
       </c>
       <c r="D94" s="12" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="95" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2482,7 +2466,7 @@
         <v>0.75</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="96" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -2496,7 +2480,7 @@
         <v>0.5</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="97" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -2510,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="98" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -2524,7 +2508,7 @@
         <v>1</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="99" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -2538,7 +2522,7 @@
         <v>1</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2552,7 +2536,7 @@
         <v>1.5</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="101" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2566,7 +2550,7 @@
         <v>1.5</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="102" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2580,7 +2564,7 @@
         <v>0.5</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="103" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2594,7 +2578,7 @@
         <v>1.5</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="150" x14ac:dyDescent="0.25">
@@ -2608,7 +2592,7 @@
         <v>1</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="105" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -2622,7 +2606,7 @@
         <v>1</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="106" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -2636,7 +2620,7 @@
         <v>1</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="107" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -2650,7 +2634,7 @@
         <v>0.5</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="108" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2664,7 +2648,7 @@
         <v>1</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="109" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2678,7 +2662,7 @@
         <v>1.5</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="110" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2692,7 +2676,7 @@
         <v>1.5</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="111" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -2706,7 +2690,7 @@
         <v>1</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2720,7 +2704,7 @@
         <v>0.75</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="113" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2734,7 +2718,7 @@
         <v>0.75</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2748,7 +2732,7 @@
         <v>1.5</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="115" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2762,7 +2746,7 @@
         <v>1.25</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="116" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2776,7 +2760,7 @@
         <v>1</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
     </row>
     <row r="117" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -2790,7 +2774,7 @@
         <v>1</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="118" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -2804,7 +2788,7 @@
         <v>1.5</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added new journal entry
</commit_message>
<xml_diff>
--- a/Coding Journal.xlsx
+++ b/Coding Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\code-journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88564A55-6F92-4621-99AE-6FC565B1C949}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39236820-15DD-42EF-81FD-DE820C0108CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0F29D09F-9D0B-41A5-94DD-0AFA6B7AA807}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="136">
   <si>
     <t>Day</t>
   </si>
@@ -1985,6 +1985,40 @@
   </si>
   <si>
     <t>InterviewCake</t>
+  </si>
+  <si>
+    <t>4/10/2020 - 4/15/2020</t>
+  </si>
+  <si>
+    <t>Update LinkedIn, Resume, Fill Out Job Applications</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FreeCodeCamp
+Front End Libraries Certification
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Quote Machine
+Added project to CodePen and made sure it passed FCC's test suite</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -2130,7 +2164,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2191,6 +2225,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2508,7 +2545,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D76F79-11B2-4973-A532-DBF6DFAAF042}">
-  <dimension ref="A1:D119"/>
+  <dimension ref="A1:D121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4178,6 +4215,28 @@
       </c>
       <c r="D119" s="9" t="s">
         <v>129</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B120" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="D120" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A121" s="18">
+        <v>116</v>
+      </c>
+      <c r="B121" s="21">
+        <v>43948</v>
+      </c>
+      <c r="C121" s="18">
+        <v>1</v>
+      </c>
+      <c r="D121" s="9" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -4212,9 +4271,10 @@
     <hyperlink ref="D117" r:id="rId27" display="https://github.com/stevegustason/quote-machine" xr:uid="{8971C486-6931-4DBD-9766-3121E14CD4E3}"/>
     <hyperlink ref="D118" r:id="rId28" display="https://github.com/stevegustason/quote-machine" xr:uid="{8CBC1B36-113D-4F95-9287-AEC94BC1B65A}"/>
     <hyperlink ref="D119" r:id="rId29" display="https://github.com/stevegustason/quote-machine" xr:uid="{09429AFE-FBA4-4D77-BE4C-948057B239F2}"/>
+    <hyperlink ref="D121" r:id="rId30" display="https://github.com/stevegustason/quote-machine" xr:uid="{FF7D3F56-7AFB-4EE3-B32D-40A908E8D226}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId30"/>
+  <pageSetup orientation="portrait" r:id="rId31"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updated code journal for 4/28
</commit_message>
<xml_diff>
--- a/Coding Journal.xlsx
+++ b/Coding Journal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\code-journal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39236820-15DD-42EF-81FD-DE820C0108CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42E474E3-4A18-4A7F-A854-55A2745FB874}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{0F29D09F-9D0B-41A5-94DD-0AFA6B7AA807}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="137">
   <si>
     <t>Day</t>
   </si>
@@ -2020,12 +2020,40 @@
 Added project to CodePen and made sure it passed FCC's test suite</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">FreeCodeCamp
+Front End Libraries Certification
+</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Markdown Previewer
+Created new React project and committed it to GitHub</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2120,8 +2148,22 @@
       <family val="2"/>
       <scheme val="major"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2130,13 +2172,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2159,10 +2206,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2196,19 +2244,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2229,8 +2274,12 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="1" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Accent3" xfId="3" builtinId="37"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Title" xfId="2" builtinId="15"/>
@@ -2545,33 +2594,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D76F79-11B2-4973-A532-DBF6DFAAF042}">
-  <dimension ref="A1:D121"/>
+  <dimension ref="A1:D122"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A116" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" style="18" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="108.42578125" style="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="18"/>
+    <col min="1" max="1" width="10.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24" style="17" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="108.42578125" style="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="17"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="17" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:4" s="16" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="12" t="s">
+      <c r="B1" s="21" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="21" t="s">
         <v>3</v>
       </c>
     </row>
@@ -2582,7 +2631,7 @@
       <c r="B2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="13"/>
+      <c r="C2" s="12"/>
       <c r="D2" s="8" t="s">
         <v>130</v>
       </c>
@@ -2980,13 +3029,13 @@
       </c>
     </row>
     <row r="31" spans="1:4" ht="135" x14ac:dyDescent="0.25">
-      <c r="A31" s="14">
+      <c r="A31" s="13">
         <v>29</v>
       </c>
-      <c r="B31" s="15">
+      <c r="B31" s="14">
         <v>43264</v>
       </c>
-      <c r="C31" s="14">
+      <c r="C31" s="13">
         <v>1</v>
       </c>
       <c r="D31" s="11" t="s">
@@ -3773,7 +3822,7 @@
       <c r="A88" s="1">
         <v>84</v>
       </c>
-      <c r="B88" s="16">
+      <c r="B88" s="15">
         <v>43894</v>
       </c>
       <c r="C88" s="2">
@@ -3787,7 +3836,7 @@
       <c r="A89" s="1">
         <v>85</v>
       </c>
-      <c r="B89" s="16">
+      <c r="B89" s="15">
         <v>43895</v>
       </c>
       <c r="C89" s="2">
@@ -3801,7 +3850,7 @@
       <c r="A90" s="1">
         <v>86</v>
       </c>
-      <c r="B90" s="16">
+      <c r="B90" s="15">
         <v>43896</v>
       </c>
       <c r="C90" s="2">
@@ -3815,7 +3864,7 @@
       <c r="A91" s="1">
         <v>87</v>
       </c>
-      <c r="B91" s="16">
+      <c r="B91" s="15">
         <v>43897</v>
       </c>
       <c r="C91" s="2">
@@ -3829,7 +3878,7 @@
       <c r="A92" s="1">
         <v>88</v>
       </c>
-      <c r="B92" s="16">
+      <c r="B92" s="15">
         <v>43898</v>
       </c>
       <c r="C92" s="2">
@@ -3843,7 +3892,7 @@
       <c r="A93" s="1">
         <v>89</v>
       </c>
-      <c r="B93" s="16">
+      <c r="B93" s="15">
         <v>43899</v>
       </c>
       <c r="C93" s="2">
@@ -3857,7 +3906,7 @@
       <c r="A94" s="1">
         <v>90</v>
       </c>
-      <c r="B94" s="16">
+      <c r="B94" s="15">
         <v>43900</v>
       </c>
       <c r="C94" s="2">
@@ -3868,13 +3917,13 @@
       </c>
     </row>
     <row r="95" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A95" s="14">
+      <c r="A95" s="13">
         <v>91</v>
       </c>
-      <c r="B95" s="15">
+      <c r="B95" s="14">
         <v>43901</v>
       </c>
-      <c r="C95" s="14">
+      <c r="C95" s="13">
         <v>3</v>
       </c>
       <c r="D95" s="11" t="s">
@@ -3885,7 +3934,7 @@
       <c r="A96" s="1">
         <v>92</v>
       </c>
-      <c r="B96" s="16">
+      <c r="B96" s="15">
         <v>43902</v>
       </c>
       <c r="C96" s="2">
@@ -3899,7 +3948,7 @@
       <c r="A97" s="1">
         <v>93</v>
       </c>
-      <c r="B97" s="16">
+      <c r="B97" s="15">
         <v>43903</v>
       </c>
       <c r="C97" s="2">
@@ -3913,7 +3962,7 @@
       <c r="A98" s="1">
         <v>94</v>
       </c>
-      <c r="B98" s="16">
+      <c r="B98" s="15">
         <v>43904</v>
       </c>
       <c r="C98" s="2">
@@ -3927,7 +3976,7 @@
       <c r="A99" s="1">
         <v>95</v>
       </c>
-      <c r="B99" s="16">
+      <c r="B99" s="15">
         <v>43905</v>
       </c>
       <c r="C99" s="2">
@@ -3941,7 +3990,7 @@
       <c r="A100" s="1">
         <v>96</v>
       </c>
-      <c r="B100" s="16">
+      <c r="B100" s="15">
         <v>43906</v>
       </c>
       <c r="C100" s="2">
@@ -3955,7 +4004,7 @@
       <c r="A101" s="1">
         <v>97</v>
       </c>
-      <c r="B101" s="16">
+      <c r="B101" s="15">
         <v>43907</v>
       </c>
       <c r="C101" s="2">
@@ -3969,7 +4018,7 @@
       <c r="A102" s="1">
         <v>98</v>
       </c>
-      <c r="B102" s="16">
+      <c r="B102" s="15">
         <v>43908</v>
       </c>
       <c r="C102" s="2">
@@ -3983,7 +4032,7 @@
       <c r="A103" s="1">
         <v>99</v>
       </c>
-      <c r="B103" s="16">
+      <c r="B103" s="15">
         <v>43909</v>
       </c>
       <c r="C103" s="2">
@@ -3997,7 +4046,7 @@
       <c r="A104" s="1">
         <v>100</v>
       </c>
-      <c r="B104" s="16">
+      <c r="B104" s="15">
         <v>43911</v>
       </c>
       <c r="C104" s="2">
@@ -4011,7 +4060,7 @@
       <c r="A105" s="1">
         <v>101</v>
       </c>
-      <c r="B105" s="16">
+      <c r="B105" s="15">
         <v>43912</v>
       </c>
       <c r="C105" s="2">
@@ -4025,7 +4074,7 @@
       <c r="A106" s="1">
         <v>102</v>
       </c>
-      <c r="B106" s="16">
+      <c r="B106" s="15">
         <v>43913</v>
       </c>
       <c r="C106" s="2">
@@ -4039,7 +4088,7 @@
       <c r="A107" s="1">
         <v>103</v>
       </c>
-      <c r="B107" s="16">
+      <c r="B107" s="15">
         <v>43914</v>
       </c>
       <c r="C107" s="2">
@@ -4053,7 +4102,7 @@
       <c r="A108" s="1">
         <v>104</v>
       </c>
-      <c r="B108" s="16">
+      <c r="B108" s="15">
         <v>43915</v>
       </c>
       <c r="C108" s="2">
@@ -4067,7 +4116,7 @@
       <c r="A109" s="1">
         <v>105</v>
       </c>
-      <c r="B109" s="16">
+      <c r="B109" s="15">
         <v>43917</v>
       </c>
       <c r="C109" s="2">
@@ -4081,7 +4130,7 @@
       <c r="A110" s="1">
         <v>106</v>
       </c>
-      <c r="B110" s="16">
+      <c r="B110" s="15">
         <v>43918</v>
       </c>
       <c r="C110" s="2">
@@ -4095,7 +4144,7 @@
       <c r="A111" s="1">
         <v>107</v>
       </c>
-      <c r="B111" s="16">
+      <c r="B111" s="15">
         <v>43920</v>
       </c>
       <c r="C111" s="2">
@@ -4109,7 +4158,7 @@
       <c r="A112" s="1">
         <v>108</v>
       </c>
-      <c r="B112" s="16">
+      <c r="B112" s="15">
         <v>43921</v>
       </c>
       <c r="C112" s="2">
@@ -4123,7 +4172,7 @@
       <c r="A113" s="1">
         <v>109</v>
       </c>
-      <c r="B113" s="16">
+      <c r="B113" s="15">
         <v>43922</v>
       </c>
       <c r="C113" s="2">
@@ -4137,7 +4186,7 @@
       <c r="A114" s="1">
         <v>110</v>
       </c>
-      <c r="B114" s="16">
+      <c r="B114" s="15">
         <v>43923</v>
       </c>
       <c r="C114" s="2">
@@ -4151,7 +4200,7 @@
       <c r="A115" s="1">
         <v>111</v>
       </c>
-      <c r="B115" s="16">
+      <c r="B115" s="15">
         <v>43926</v>
       </c>
       <c r="C115" s="2">
@@ -4165,7 +4214,7 @@
       <c r="A116" s="1">
         <v>112</v>
       </c>
-      <c r="B116" s="16">
+      <c r="B116" s="15">
         <v>43927</v>
       </c>
       <c r="C116" s="2">
@@ -4179,7 +4228,7 @@
       <c r="A117" s="1">
         <v>113</v>
       </c>
-      <c r="B117" s="16">
+      <c r="B117" s="15">
         <v>43928</v>
       </c>
       <c r="C117" s="2">
@@ -4193,7 +4242,7 @@
       <c r="A118" s="1">
         <v>114</v>
       </c>
-      <c r="B118" s="16">
+      <c r="B118" s="15">
         <v>43929</v>
       </c>
       <c r="C118" s="2">
@@ -4207,7 +4256,7 @@
       <c r="A119" s="1">
         <v>115</v>
       </c>
-      <c r="B119" s="16">
+      <c r="B119" s="15">
         <v>43930</v>
       </c>
       <c r="C119" s="2">
@@ -4218,25 +4267,39 @@
       </c>
     </row>
     <row r="120" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B120" s="18" t="s">
+      <c r="B120" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="D120" s="18" t="s">
+      <c r="D120" s="17" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="121" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A121" s="18">
+      <c r="A121" s="17">
         <v>116</v>
       </c>
-      <c r="B121" s="21">
+      <c r="B121" s="20">
         <v>43948</v>
       </c>
-      <c r="C121" s="18">
+      <c r="C121" s="17">
         <v>1</v>
       </c>
       <c r="D121" s="9" t="s">
         <v>135</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A122" s="17">
+        <v>117</v>
+      </c>
+      <c r="B122" s="20">
+        <v>43949</v>
+      </c>
+      <c r="C122" s="17">
+        <v>0.5</v>
+      </c>
+      <c r="D122" s="9" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -4272,9 +4335,10 @@
     <hyperlink ref="D118" r:id="rId28" display="https://github.com/stevegustason/quote-machine" xr:uid="{8CBC1B36-113D-4F95-9287-AEC94BC1B65A}"/>
     <hyperlink ref="D119" r:id="rId29" display="https://github.com/stevegustason/quote-machine" xr:uid="{09429AFE-FBA4-4D77-BE4C-948057B239F2}"/>
     <hyperlink ref="D121" r:id="rId30" display="https://github.com/stevegustason/quote-machine" xr:uid="{FF7D3F56-7AFB-4EE3-B32D-40A908E8D226}"/>
+    <hyperlink ref="D122" r:id="rId31" display="https://github.com/stevegustason/markdown-previewer" xr:uid="{5980E1A7-03A2-4880-AE1F-B15FC97A59CF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId31"/>
+  <pageSetup orientation="portrait" r:id="rId32"/>
 </worksheet>
 </file>
 
@@ -4293,17 +4357,17 @@
     <col min="5" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="20" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:4" s="19" customFormat="1" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="18" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>